<commit_message>
ADD: updated supp. tables
</commit_message>
<xml_diff>
--- a/data/final/data_dictionary_anomaly_v20240806.xlsx
+++ b/data/final/data_dictionary_anomaly_v20240806.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamova/Documents/projects/14_LM1/NJODE/Probabilistic_forecasting_for_Anomaly_Detection/data/original_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamova/Documents/projects/14_LM1/NJODE/anomaly_microbiome_data_processing/data/final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A71D4C-FF85-7E4C-B874-DD7D33E362CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E3FA6E-915E-CC48-BF38-531CB4D71CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22300" yWindow="860" windowWidth="22840" windowHeight="18560" xr2:uid="{0751DAF1-5C18-FB4D-876E-E89AC4BC8475}"/>
+    <workbookView xWindow="19600" yWindow="2760" windowWidth="22840" windowHeight="18560" xr2:uid="{0751DAF1-5C18-FB4D-876E-E89AC4BC8475}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
-    <sheet name="ft_vat19_anomaly_v{}_entero_fam" sheetId="5" r:id="rId2"/>
-    <sheet name="ft_vat19_anomaly_v{}_entero_gen" sheetId="7" r:id="rId3"/>
+    <sheet name="ft_vat19_anomaly_v{}_entero_gen" sheetId="7" r:id="rId2"/>
+    <sheet name="ft_vat19_anomaly_v{}_entero_fam" sheetId="5" r:id="rId3"/>
     <sheet name="ts_vat19_abx_v{}" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ft_vat19_anomaly_v{}_entero_fam'!$A$1:$F$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ft_vat19_anomaly_v{}_entero_gen'!$A$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ft_vat19_anomaly_v{}_entero_fam'!$A$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ft_vat19_anomaly_v{}_entero_gen'!$A$1:$F$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Description of the field.</t>
   </si>
   <si>
-    <t>Suggested usage of this field for anomaly detection usecase.</t>
-  </si>
-  <si>
     <t>Age of infant in days at time of sampling.</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>[0.0, 0.996288]</t>
   </si>
   <si>
-    <t>Microbial feature for enteropathogens</t>
-  </si>
-  <si>
     <t>rel_abd_enteropathogens_genus</t>
   </si>
   <si>
@@ -349,6 +343,9 @@
   </si>
   <si>
     <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Usage of this field for anomaly detection usecase.</t>
   </si>
   <si>
     <r>
@@ -374,6 +371,26 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">for the processed microbiome datasets for the anomaly detection usecase with PD-NJ-ODE. Each dataset is described in a separate Excel sheet: 
+* </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>"ft_vat19_anomaly_v{}_entero_genus"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Feature table containing metadata, alpha diversity and relative abundances of enteropathogens grouped on genus level for each sample. Only metdata and alpha diversity values were used for modelling.
 * </t>
     </r>
     <r>
@@ -404,49 +421,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Feature table containing metadata, alpha diversity and relative abundances of enteropathogens grouped on family level for each sample. 
-* </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>ft_vat19_anomaly_v{}_entero_genus</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Feature table containing metadata, alpha diversity and relative abundances of enteropathogens grouped on genus level for each sample. 
+      <t xml:space="preserve"> Feature table containing metadata, alpha diversity and relative abundances of enteropathogens grouped on family level for each sample - not used for modelling.
 * </t>
     </r>
     <r>
@@ -506,7 +481,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,14 +527,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="4"/>
       <name val="Calibri (Body)"/>
     </font>
@@ -584,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -610,10 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -932,7 +895,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J6"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -942,7 +905,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1115,7 +1078,7 @@
         <v>46</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1262,15 +1225,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B027464-B3C2-F546-9B60-5A13195C6419}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3589B3D5-3732-2643-977F-AE8CFEC13C8A}">
   <sheetPr>
-    <tabColor rgb="FF7030A0"/>
+    <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1335,7 +1298,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>48</v>
@@ -1355,7 +1318,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>47</v>
@@ -1378,7 +1341,7 @@
         <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1398,7 +1361,7 @@
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1418,7 +1381,7 @@
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -1438,7 +1401,7 @@
         <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1458,12 +1421,12 @@
         <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>43</v>
@@ -1483,7 +1446,7 @@
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>43</v>
@@ -1495,7 +1458,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>48</v>
@@ -1603,7 +1566,7 @@
     </row>
     <row r="17" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
@@ -1612,18 +1575,18 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
@@ -1632,18 +1595,18 @@
         <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
@@ -1652,38 +1615,38 @@
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
@@ -1692,13 +1655,13 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1708,15 +1671,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3589B3D5-3732-2643-977F-AE8CFEC13C8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B027464-B3C2-F546-9B60-5A13195C6419}">
   <sheetPr>
-    <tabColor theme="9" tint="-0.249977111117893"/>
+    <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1781,7 +1744,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>48</v>
@@ -1801,7 +1764,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>47</v>
@@ -1824,7 +1787,7 @@
         <v>32</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1844,7 +1807,7 @@
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1864,7 +1827,7 @@
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -1884,7 +1847,7 @@
         <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1904,12 +1867,12 @@
         <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>43</v>
@@ -1929,7 +1892,7 @@
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>43</v>
@@ -1941,7 +1904,7 @@
         <v>44</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>48</v>
@@ -2049,7 +2012,7 @@
     </row>
     <row r="17" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
@@ -2058,18 +2021,18 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>6</v>
@@ -2078,18 +2041,18 @@
         <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
@@ -2098,38 +2061,38 @@
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="187" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
@@ -2138,13 +2101,13 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2206,7 +2169,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>47</v>
@@ -2223,13 +2186,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -2246,17 +2209,17 @@
         <v>54</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2265,18 +2228,18 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="11" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2285,11 +2248,11 @@
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>101</v>
+      <c r="E6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>